<commit_message>
interface modificada e backend acertado(revisar)
</commit_message>
<xml_diff>
--- a/teste/1.xlsx
+++ b/teste/1.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vendas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,17 +27,23 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,20 +51,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,6 +432,77 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="21" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="17" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="13" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="21" customWidth="1" min="21" max="21"/>
+    <col width="17" customWidth="1" min="22" max="22"/>
+    <col width="22" customWidth="1" min="23" max="23"/>
+    <col width="17" customWidth="1" min="24" max="24"/>
+    <col width="20" customWidth="1" min="25" max="25"/>
+    <col width="14" customWidth="1" min="26" max="26"/>
+    <col width="13" customWidth="1" min="27" max="27"/>
+    <col width="19" customWidth="1" min="28" max="28"/>
+    <col width="17" customWidth="1" min="29" max="29"/>
+    <col width="23" customWidth="1" min="30" max="30"/>
+    <col width="19" customWidth="1" min="31" max="31"/>
+    <col width="16" customWidth="1" min="32" max="32"/>
+    <col width="19" customWidth="1" min="33" max="33"/>
+    <col width="12" customWidth="1" min="34" max="34"/>
+    <col width="12" customWidth="1" min="35" max="35"/>
+    <col width="12" customWidth="1" min="36" max="36"/>
+    <col width="12" customWidth="1" min="37" max="37"/>
+    <col width="12" customWidth="1" min="38" max="38"/>
+    <col width="12" customWidth="1" min="39" max="39"/>
+    <col width="13" customWidth="1" min="40" max="40"/>
+    <col width="12" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="26" customWidth="1" min="45" max="45"/>
+    <col width="13" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="15" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="12" customWidth="1" min="50" max="50"/>
+    <col width="12" customWidth="1" min="51" max="51"/>
+    <col width="14" customWidth="1" min="52" max="52"/>
+    <col width="12" customWidth="1" min="53" max="53"/>
+    <col width="12" customWidth="1" min="54" max="54"/>
+    <col width="13" customWidth="1" min="55" max="55"/>
+    <col width="17" customWidth="1" min="56" max="56"/>
+    <col width="14" customWidth="1" min="57" max="57"/>
+    <col width="12" customWidth="1" min="58" max="58"/>
+    <col width="16" customWidth="1" min="59" max="59"/>
+    <col width="16" customWidth="1" min="60" max="60"/>
+    <col width="12" customWidth="1" min="61" max="61"/>
+    <col width="14" customWidth="1" min="62" max="62"/>
+    <col width="12" customWidth="1" min="63" max="63"/>
+    <col width="26" customWidth="1" min="64" max="64"/>
+    <col width="17" customWidth="1" min="65" max="65"/>
+    <col width="12" customWidth="1" min="66" max="66"/>
+    <col width="12" customWidth="1" min="67" max="67"/>
+    <col width="22" customWidth="1" min="68" max="68"/>
+    <col width="28" customWidth="1" min="69" max="69"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>